<commit_message>
Update links and refine countdown/share-reminder UI states
</commit_message>
<xml_diff>
--- a/docs/データベース.xlsx
+++ b/docs/データベース.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yana/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yana/Downloads/VoiceTree/HP作成/260221_PICKUPLIVER/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{458ABE6E-BBE0-1845-989B-CB8904349DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162EDEA8-23FE-A54E-A793-04766E70D5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="820" windowWidth="28300" windowHeight="17360" xr2:uid="{2141F815-2034-6D42-8FA2-D8076E8BD180}"/>
   </bookViews>
@@ -101,10 +101,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://web.colorsing.com/share/live?live_id=1911fb37-2653-4a0b-a797-86d47697b83b</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>https://web.colorsing.com/share/user?user_id=91910bec-747b-4b6d-9882-8cf363242c7e</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -133,6 +129,10 @@
     <rPh sb="0" eb="2">
       <t>ハイシn</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://web.colorsing.com/share/user?user_id=6df8aef6-db3d-4609-898e-d1a610954a8b</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -528,7 +528,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -555,7 +555,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -566,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -577,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -588,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -599,7 +599,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -610,7 +610,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -621,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>